<commit_message>
Update AlgoHives_Score.xlsx with new scoring data
</commit_message>
<xml_diff>
--- a/AlgoHives_Score.xlsx
+++ b/AlgoHives_Score.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ericp\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85229D6-CE44-4323-9B25-78477877350A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A40192-00FD-4A71-AD3C-A619DF19474F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{43B1E640-5D66-4AA2-865F-F50210FF57CA}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
   <si>
     <t>EASY</t>
   </si>
@@ -167,9 +167,6 @@
   </si>
   <si>
     <t>VARIABLES</t>
-  </si>
-  <si>
-    <t>EASY1</t>
   </si>
   <si>
     <t>ATTEMPTS</t>
@@ -763,7 +760,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -802,7 +799,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="B2" s="8">
         <v>1</v>
@@ -899,7 +896,7 @@
       </c>
       <c r="D6" s="11"/>
       <c r="G6" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Update AlgoHives_Score.xlsx with revised scoring data
</commit_message>
<xml_diff>
--- a/AlgoHives_Score.xlsx
+++ b/AlgoHives_Score.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ericp\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\ericp\AlgoHive\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A40192-00FD-4A71-AD3C-A619DF19474F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D28501-53CE-48A2-BCDB-0FDCF059FEF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{43B1E640-5D66-4AA2-865F-F50210FF57CA}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
   <si>
     <t>EASY</t>
   </si>
@@ -170,6 +170,30 @@
   </si>
   <si>
     <t>ATTEMPTS</t>
+  </si>
+  <si>
+    <t>MAXIMUM</t>
+  </si>
+  <si>
+    <t>MAX_TWO_PARTS</t>
+  </si>
+  <si>
+    <t>MOYENNE</t>
+  </si>
+  <si>
+    <t>MAXIMUM NOTE</t>
+  </si>
+  <si>
+    <t>FINAL_SCORE</t>
+  </si>
+  <si>
+    <t>GRADE</t>
+  </si>
+  <si>
+    <t>Valeur Utilisateur :</t>
+  </si>
+  <si>
+    <t>&lt;------   /!\ GRADE User calculée automatiquement /!\</t>
   </si>
 </sst>
 </file>
@@ -210,7 +234,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -271,8 +295,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -365,11 +407,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -437,6 +492,36 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -757,14 +842,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73D0CB78-860A-4C75-B2F5-CDDF66AFB44E}">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50:H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="17.5546875" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.77734375" style="1" customWidth="1"/>
     <col min="4" max="4" width="1.88671875" customWidth="1"/>
@@ -1176,8 +1262,321 @@
       <c r="C32" s="12"/>
       <c r="D32" s="11"/>
     </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="26"/>
+      <c r="D33" s="11"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>1</v>
+      </c>
+      <c r="B34" s="22">
+        <f>((C2+C15)*1.01) + ((C3+C15)*1.01)</f>
+        <v>90.9</v>
+      </c>
+      <c r="C34" s="22"/>
+      <c r="D34" s="11"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
+        <v>2</v>
+      </c>
+      <c r="B35" s="22">
+        <f>((C2+C15)*1.02) + ((C3+C15)*1.02)</f>
+        <v>91.800000000000011</v>
+      </c>
+      <c r="C35" s="22"/>
+      <c r="D35" s="11"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
+        <v>3</v>
+      </c>
+      <c r="B36" s="22">
+        <f>((C2+C15)*1.03) + ((C3+C15)*1.03)</f>
+        <v>92.7</v>
+      </c>
+      <c r="C36" s="22"/>
+      <c r="D36" s="11"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
+        <v>4</v>
+      </c>
+      <c r="B37" s="22">
+        <f>((C2+C15)*1.04) + ((C3+C15)*1.04)</f>
+        <v>93.6</v>
+      </c>
+      <c r="C37" s="22"/>
+      <c r="D37" s="11"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
+        <v>5</v>
+      </c>
+      <c r="B38" s="22">
+        <f>((C2+C15)*1.05) + ((C3+C15)*1.05)</f>
+        <v>94.5</v>
+      </c>
+      <c r="C38" s="22"/>
+      <c r="D38" s="11"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
+        <v>6</v>
+      </c>
+      <c r="B39" s="22">
+        <f>((C4+C18)*1.06) + ((C5+C18)*1.06)</f>
+        <v>148.4</v>
+      </c>
+      <c r="C39" s="22"/>
+      <c r="D39" s="11"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
+        <v>7</v>
+      </c>
+      <c r="B40" s="22">
+        <f>((C4+C18)*1.07) + ((C5+C18)*1.07)</f>
+        <v>149.80000000000001</v>
+      </c>
+      <c r="C40" s="22"/>
+      <c r="D40" s="11"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="2">
+        <v>8</v>
+      </c>
+      <c r="B41" s="22">
+        <f>((C4+C18)*1.08) + ((C5+C18)*1.08)</f>
+        <v>151.20000000000002</v>
+      </c>
+      <c r="C41" s="22"/>
+      <c r="D41" s="11"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="2">
+        <v>9</v>
+      </c>
+      <c r="B42" s="22">
+        <f>((C4+C18)*1.09) + ((C5+C18)*1.09)</f>
+        <v>152.60000000000002</v>
+      </c>
+      <c r="C42" s="22"/>
+      <c r="D42" s="11"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="2">
+        <v>10</v>
+      </c>
+      <c r="B43" s="22">
+        <f>((C4+C18)*1.1) + ((C5+C18)*1.1)</f>
+        <v>154.00000000000003</v>
+      </c>
+      <c r="C43" s="22"/>
+      <c r="D43" s="11"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="2">
+        <v>11</v>
+      </c>
+      <c r="B44" s="22">
+        <f>((C4+C18)*1.11) + ((C5+C18)*1.11)</f>
+        <v>155.4</v>
+      </c>
+      <c r="C44" s="22"/>
+      <c r="D44" s="11"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
+        <v>12</v>
+      </c>
+      <c r="B45" s="22">
+        <f>((C6+C21)*1.12) + ((C7+C21)*1.12)</f>
+        <v>392</v>
+      </c>
+      <c r="C45" s="22"/>
+      <c r="D45" s="11"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="2">
+        <v>13</v>
+      </c>
+      <c r="B46" s="22">
+        <f>((C6+C21)*1.13) + ((C7+C21)*1.13)</f>
+        <v>395.5</v>
+      </c>
+      <c r="C46" s="22"/>
+      <c r="D46" s="11"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="2">
+        <v>14</v>
+      </c>
+      <c r="B47" s="22">
+        <f>((C6+C21)*1.14) + ((C7+C21)*1.14)</f>
+        <v>399</v>
+      </c>
+      <c r="C47" s="22"/>
+      <c r="D47" s="11"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="2">
+        <v>15</v>
+      </c>
+      <c r="B48" s="22">
+        <f>((C6+C21)*1.15) + ((C7+C21)*1.15)</f>
+        <v>402.5</v>
+      </c>
+      <c r="C48" s="22"/>
+      <c r="D48" s="11"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" s="2">
+        <v>16</v>
+      </c>
+      <c r="B49" s="22">
+        <f>((C6+C21)*1.16) + ((C7+C21)*1.16)</f>
+        <v>406</v>
+      </c>
+      <c r="C49" s="22"/>
+      <c r="D49" s="11"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B50" s="32">
+        <f>SUM(B34:B38)</f>
+        <v>463.5</v>
+      </c>
+      <c r="C50" s="32"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="24"/>
+      <c r="F50" s="24"/>
+      <c r="G50" s="24"/>
+      <c r="H50" s="24"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B51" s="30">
+        <f>SUM(B34:B43)</f>
+        <v>1219.5</v>
+      </c>
+      <c r="C51" s="30"/>
+      <c r="D51" s="11"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B52" s="28">
+        <f>SUM(B34:B49)</f>
+        <v>3369.9</v>
+      </c>
+      <c r="C52" s="28"/>
+      <c r="D52" s="11"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" s="11"/>
+      <c r="B53" s="12"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="11"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" s="35"/>
+      <c r="B54" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D54" s="11"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="B55" s="20">
+        <v>438</v>
+      </c>
+      <c r="C55" s="20">
+        <f>MIN(20, ROUNDUP(IF(B55&lt;=470, (B55/470)*10, 10 + ((B55-470)/(1219.5-470))*10), 0.5))</f>
+        <v>10</v>
+      </c>
+      <c r="D55" s="11"/>
+      <c r="E55" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="F55" s="37"/>
+      <c r="G55" s="37"/>
+      <c r="H55" s="37"/>
+      <c r="I55" s="37"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="B56" s="34">
+        <f>SUM(B34:B41)</f>
+        <v>912.90000000000009</v>
+      </c>
+      <c r="C56" s="34">
+        <v>10</v>
+      </c>
+      <c r="D56" s="11"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B57" s="34">
+        <f>SUM(B34:B45)</f>
+        <v>1766.9</v>
+      </c>
+      <c r="C57" s="34">
+        <v>20</v>
+      </c>
+      <c r="D57" s="11"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58" s="12"/>
+      <c r="B58" s="12"/>
+      <c r="C58" s="12"/>
+      <c r="D58" s="11"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="28">
+    <mergeCell ref="E55:I55"/>
+    <mergeCell ref="E50:H50"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
     <mergeCell ref="A31:C31"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B27:C27"/>

</xml_diff>

<commit_message>
Update AlgoHives_Score.xlsx with modified scoring data
</commit_message>
<xml_diff>
--- a/AlgoHives_Score.xlsx
+++ b/AlgoHives_Score.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\ericp\AlgoHive\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D28501-53CE-48A2-BCDB-0FDCF059FEF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC849DD-716D-4CA7-A880-375310FDD1C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{43B1E640-5D66-4AA2-865F-F50210FF57CA}"/>
   </bookViews>
@@ -484,36 +484,9 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -522,6 +495,33 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -844,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73D0CB78-860A-4C75-B2F5-CDDF66AFB44E}">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50:H50"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1204,56 +1204,56 @@
       <c r="A26" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="22" t="s">
+      <c r="B26" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="22"/>
+      <c r="C26" s="30"/>
       <c r="D26" s="11"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="16">
         <v>1</v>
       </c>
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="22"/>
+      <c r="C27" s="30"/>
       <c r="D27" s="11"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="16">
         <v>2</v>
       </c>
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="22"/>
+      <c r="C28" s="30"/>
       <c r="D28" s="11"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="23" t="s">
+      <c r="A29" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
       <c r="D29" s="11"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="16">
         <v>10</v>
       </c>
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="22"/>
+      <c r="C30" s="30"/>
       <c r="D30" s="11"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="21" t="s">
+      <c r="A31" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="36"/>
       <c r="D31" s="11"/>
     </row>
     <row r="32" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.3">
@@ -1266,223 +1266,222 @@
       <c r="A33" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="25" t="s">
+      <c r="B33" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C33" s="26"/>
+      <c r="C33" s="35"/>
       <c r="D33" s="11"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>1</v>
       </c>
-      <c r="B34" s="22">
+      <c r="B34" s="30">
         <f>((C2+C15)*1.01) + ((C3+C15)*1.01)</f>
         <v>90.9</v>
       </c>
-      <c r="C34" s="22"/>
+      <c r="C34" s="30"/>
       <c r="D34" s="11"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>2</v>
       </c>
-      <c r="B35" s="22">
+      <c r="B35" s="30">
         <f>((C2+C15)*1.02) + ((C3+C15)*1.02)</f>
         <v>91.800000000000011</v>
       </c>
-      <c r="C35" s="22"/>
+      <c r="C35" s="30"/>
       <c r="D35" s="11"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>3</v>
       </c>
-      <c r="B36" s="22">
+      <c r="B36" s="30">
         <f>((C2+C15)*1.03) + ((C3+C15)*1.03)</f>
         <v>92.7</v>
       </c>
-      <c r="C36" s="22"/>
+      <c r="C36" s="30"/>
       <c r="D36" s="11"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>4</v>
       </c>
-      <c r="B37" s="22">
+      <c r="B37" s="30">
         <f>((C2+C15)*1.04) + ((C3+C15)*1.04)</f>
         <v>93.6</v>
       </c>
-      <c r="C37" s="22"/>
+      <c r="C37" s="30"/>
       <c r="D37" s="11"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>5</v>
       </c>
-      <c r="B38" s="22">
+      <c r="B38" s="30">
         <f>((C2+C15)*1.05) + ((C3+C15)*1.05)</f>
         <v>94.5</v>
       </c>
-      <c r="C38" s="22"/>
+      <c r="C38" s="30"/>
       <c r="D38" s="11"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>6</v>
       </c>
-      <c r="B39" s="22">
+      <c r="B39" s="30">
         <f>((C4+C18)*1.06) + ((C5+C18)*1.06)</f>
         <v>148.4</v>
       </c>
-      <c r="C39" s="22"/>
+      <c r="C39" s="30"/>
       <c r="D39" s="11"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>7</v>
       </c>
-      <c r="B40" s="22">
+      <c r="B40" s="30">
         <f>((C4+C18)*1.07) + ((C5+C18)*1.07)</f>
         <v>149.80000000000001</v>
       </c>
-      <c r="C40" s="22"/>
+      <c r="C40" s="30"/>
       <c r="D40" s="11"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>8</v>
       </c>
-      <c r="B41" s="22">
+      <c r="B41" s="30">
         <f>((C4+C18)*1.08) + ((C5+C18)*1.08)</f>
         <v>151.20000000000002</v>
       </c>
-      <c r="C41" s="22"/>
+      <c r="C41" s="30"/>
       <c r="D41" s="11"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>9</v>
       </c>
-      <c r="B42" s="22">
+      <c r="B42" s="30">
         <f>((C4+C18)*1.09) + ((C5+C18)*1.09)</f>
         <v>152.60000000000002</v>
       </c>
-      <c r="C42" s="22"/>
+      <c r="C42" s="30"/>
       <c r="D42" s="11"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>10</v>
       </c>
-      <c r="B43" s="22">
+      <c r="B43" s="30">
         <f>((C4+C18)*1.1) + ((C5+C18)*1.1)</f>
         <v>154.00000000000003</v>
       </c>
-      <c r="C43" s="22"/>
+      <c r="C43" s="30"/>
       <c r="D43" s="11"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>11</v>
       </c>
-      <c r="B44" s="22">
+      <c r="B44" s="30">
         <f>((C4+C18)*1.11) + ((C5+C18)*1.11)</f>
         <v>155.4</v>
       </c>
-      <c r="C44" s="22"/>
+      <c r="C44" s="30"/>
       <c r="D44" s="11"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>12</v>
       </c>
-      <c r="B45" s="22">
+      <c r="B45" s="30">
         <f>((C6+C21)*1.12) + ((C7+C21)*1.12)</f>
         <v>392</v>
       </c>
-      <c r="C45" s="22"/>
+      <c r="C45" s="30"/>
       <c r="D45" s="11"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>13</v>
       </c>
-      <c r="B46" s="22">
+      <c r="B46" s="30">
         <f>((C6+C21)*1.13) + ((C7+C21)*1.13)</f>
         <v>395.5</v>
       </c>
-      <c r="C46" s="22"/>
+      <c r="C46" s="30"/>
       <c r="D46" s="11"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>14</v>
       </c>
-      <c r="B47" s="22">
+      <c r="B47" s="30">
         <f>((C6+C21)*1.14) + ((C7+C21)*1.14)</f>
         <v>399</v>
       </c>
-      <c r="C47" s="22"/>
+      <c r="C47" s="30"/>
       <c r="D47" s="11"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>15</v>
       </c>
-      <c r="B48" s="22">
+      <c r="B48" s="30">
         <f>((C6+C21)*1.15) + ((C7+C21)*1.15)</f>
         <v>402.5</v>
       </c>
-      <c r="C48" s="22"/>
+      <c r="C48" s="30"/>
       <c r="D48" s="11"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>16</v>
       </c>
-      <c r="B49" s="22">
+      <c r="B49" s="30">
         <f>((C6+C21)*1.16) + ((C7+C21)*1.16)</f>
         <v>406</v>
       </c>
-      <c r="C49" s="22"/>
+      <c r="C49" s="30"/>
       <c r="D49" s="11"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="31" t="s">
+      <c r="A50" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="B50" s="32">
-        <f>SUM(B34:B38)</f>
-        <v>463.5</v>
-      </c>
-      <c r="C50" s="32"/>
+      <c r="B50" s="31">
+        <v>470</v>
+      </c>
+      <c r="C50" s="31"/>
       <c r="D50" s="11"/>
-      <c r="E50" s="24"/>
-      <c r="F50" s="24"/>
-      <c r="G50" s="24"/>
-      <c r="H50" s="24"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="29"/>
+      <c r="G50" s="29"/>
+      <c r="H50" s="29"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="29" t="s">
+      <c r="A51" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="B51" s="30">
+      <c r="B51" s="32">
         <f>SUM(B34:B43)</f>
         <v>1219.5</v>
       </c>
-      <c r="C51" s="30"/>
+      <c r="C51" s="32"/>
       <c r="D51" s="11"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="27" t="s">
+      <c r="A52" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="B52" s="28">
+      <c r="B52" s="33">
         <f>SUM(B34:B49)</f>
         <v>3369.9</v>
       </c>
-      <c r="C52" s="28"/>
+      <c r="C52" s="33"/>
       <c r="D52" s="11"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
@@ -1492,7 +1491,7 @@
       <c r="D53" s="11"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="35"/>
+      <c r="A54" s="26"/>
       <c r="B54" s="4" t="s">
         <v>42</v>
       </c>
@@ -1502,47 +1501,47 @@
       <c r="D54" s="11"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="36" t="s">
+      <c r="A55" s="27" t="s">
         <v>44</v>
       </c>
       <c r="B55" s="20">
-        <v>438</v>
+        <v>1220</v>
       </c>
       <c r="C55" s="20">
         <f>MIN(20, ROUNDUP(IF(B55&lt;=470, (B55/470)*10, 10 + ((B55-470)/(1219.5-470))*10), 0.5))</f>
+        <v>20</v>
+      </c>
+      <c r="D55" s="11"/>
+      <c r="E55" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="F55" s="28"/>
+      <c r="G55" s="28"/>
+      <c r="H55" s="28"/>
+      <c r="I55" s="28"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B56" s="25">
+        <f>B50</f>
+        <v>470</v>
+      </c>
+      <c r="C56" s="25">
         <v>10</v>
       </c>
-      <c r="D55" s="11"/>
-      <c r="E55" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="F55" s="37"/>
-      <c r="G55" s="37"/>
-      <c r="H55" s="37"/>
-      <c r="I55" s="37"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B56" s="34">
-        <f>SUM(B34:B41)</f>
-        <v>912.90000000000009</v>
-      </c>
-      <c r="C56" s="34">
-        <v>10</v>
-      </c>
       <c r="D56" s="11"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="33" t="s">
+      <c r="A57" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="B57" s="34">
-        <f>SUM(B34:B45)</f>
-        <v>1766.9</v>
-      </c>
-      <c r="C57" s="34">
+      <c r="B57" s="25">
+        <f>B51</f>
+        <v>1219.5</v>
+      </c>
+      <c r="C57" s="25">
         <v>20</v>
       </c>
       <c r="D57" s="11"/>
@@ -1555,6 +1554,27 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
     <mergeCell ref="E55:I55"/>
     <mergeCell ref="E50:H50"/>
     <mergeCell ref="B48:C48"/>
@@ -1562,27 +1582,6 @@
     <mergeCell ref="B50:C50"/>
     <mergeCell ref="B51:C51"/>
     <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="A29:C29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update AlgoHives_Score.xlsx with updated scoring data
</commit_message>
<xml_diff>
--- a/AlgoHives_Score.xlsx
+++ b/AlgoHives_Score.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\ericp\AlgoHive\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC849DD-716D-4CA7-A880-375310FDD1C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB0AA76-C16E-443E-8F4E-DBBBF54DDD61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{43B1E640-5D66-4AA2-865F-F50210FF57CA}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
   <si>
     <t>EASY</t>
   </si>
@@ -493,15 +493,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -509,18 +521,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -844,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73D0CB78-860A-4C75-B2F5-CDDF66AFB44E}">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -898,7 +898,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I2" s="18">
         <v>0</v>
@@ -923,7 +923,7 @@
       </c>
       <c r="I3" s="18" cm="1">
         <f t="array" ref="I3">_xlfn.XLOOKUP(H2&amp;H3,A2:A7&amp;B2:B7,C2:C7,0,)</f>
-        <v>135</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -941,11 +941,11 @@
         <v>31</v>
       </c>
       <c r="H4" s="2">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="I4" s="18" t="str">
         <f>_xlfn.CONCAT("1.",IF((H4)&lt;10,_xlfn.CONCAT("0",H4),H4))</f>
-        <v>1.16</v>
+        <v>1.09</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -963,11 +963,11 @@
         <v>32</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I5" s="18" cm="1">
         <f t="array" ref="I5">_xlfn.XLOOKUP(H2&amp;H5,A15:A23&amp;B15:B23,C15:C23,0,)</f>
-        <v>75</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -984,12 +984,12 @@
       <c r="G6" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>8</v>
+      <c r="H6" s="2">
+        <v>0</v>
       </c>
       <c r="I6" s="18">
         <f>_xlfn.XLOOKUP(H6,A10:A12,B10:B12,0,)</f>
-        <v>-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -1008,7 +1008,7 @@
       </c>
       <c r="H7" s="20">
         <f>(I3+I5+I6)*I4</f>
-        <v>241.27999999999997</v>
+        <v>92.65</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="8.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1204,56 +1204,56 @@
       <c r="A26" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="30"/>
+      <c r="C26" s="29"/>
       <c r="D26" s="11"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="16">
         <v>1</v>
       </c>
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="30"/>
+      <c r="C27" s="29"/>
       <c r="D27" s="11"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="16">
         <v>2</v>
       </c>
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="30"/>
+      <c r="C28" s="29"/>
       <c r="D28" s="11"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
       <c r="D29" s="11"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="16">
         <v>10</v>
       </c>
-      <c r="B30" s="30" t="s">
+      <c r="B30" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="30"/>
+      <c r="C30" s="29"/>
       <c r="D30" s="11"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="36" t="s">
+      <c r="A31" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="36"/>
-      <c r="C31" s="36"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
       <c r="D31" s="11"/>
     </row>
     <row r="32" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.3">
@@ -1266,222 +1266,223 @@
       <c r="A33" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="34" t="s">
+      <c r="B33" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="C33" s="35"/>
+      <c r="C33" s="32"/>
       <c r="D33" s="11"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>1</v>
       </c>
-      <c r="B34" s="30">
+      <c r="B34" s="29">
         <f>((C2+C15)*1.01) + ((C3+C15)*1.01)</f>
         <v>90.9</v>
       </c>
-      <c r="C34" s="30"/>
+      <c r="C34" s="29"/>
       <c r="D34" s="11"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>2</v>
       </c>
-      <c r="B35" s="30">
+      <c r="B35" s="29">
         <f>((C2+C15)*1.02) + ((C3+C15)*1.02)</f>
         <v>91.800000000000011</v>
       </c>
-      <c r="C35" s="30"/>
+      <c r="C35" s="29"/>
       <c r="D35" s="11"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>3</v>
       </c>
-      <c r="B36" s="30">
+      <c r="B36" s="29">
         <f>((C2+C15)*1.03) + ((C3+C15)*1.03)</f>
         <v>92.7</v>
       </c>
-      <c r="C36" s="30"/>
+      <c r="C36" s="29"/>
       <c r="D36" s="11"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>4</v>
       </c>
-      <c r="B37" s="30">
+      <c r="B37" s="29">
         <f>((C2+C15)*1.04) + ((C3+C15)*1.04)</f>
         <v>93.6</v>
       </c>
-      <c r="C37" s="30"/>
+      <c r="C37" s="29"/>
       <c r="D37" s="11"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>5</v>
       </c>
-      <c r="B38" s="30">
+      <c r="B38" s="29">
         <f>((C2+C15)*1.05) + ((C3+C15)*1.05)</f>
         <v>94.5</v>
       </c>
-      <c r="C38" s="30"/>
+      <c r="C38" s="29"/>
       <c r="D38" s="11"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>6</v>
       </c>
-      <c r="B39" s="30">
+      <c r="B39" s="29">
         <f>((C4+C18)*1.06) + ((C5+C18)*1.06)</f>
         <v>148.4</v>
       </c>
-      <c r="C39" s="30"/>
+      <c r="C39" s="29"/>
       <c r="D39" s="11"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>7</v>
       </c>
-      <c r="B40" s="30">
+      <c r="B40" s="29">
         <f>((C4+C18)*1.07) + ((C5+C18)*1.07)</f>
         <v>149.80000000000001</v>
       </c>
-      <c r="C40" s="30"/>
+      <c r="C40" s="29"/>
       <c r="D40" s="11"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>8</v>
       </c>
-      <c r="B41" s="30">
+      <c r="B41" s="29">
         <f>((C4+C18)*1.08) + ((C5+C18)*1.08)</f>
         <v>151.20000000000002</v>
       </c>
-      <c r="C41" s="30"/>
+      <c r="C41" s="29"/>
       <c r="D41" s="11"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>9</v>
       </c>
-      <c r="B42" s="30">
+      <c r="B42" s="29">
         <f>((C4+C18)*1.09) + ((C5+C18)*1.09)</f>
         <v>152.60000000000002</v>
       </c>
-      <c r="C42" s="30"/>
+      <c r="C42" s="29"/>
       <c r="D42" s="11"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>10</v>
       </c>
-      <c r="B43" s="30">
+      <c r="B43" s="29">
         <f>((C4+C18)*1.1) + ((C5+C18)*1.1)</f>
         <v>154.00000000000003</v>
       </c>
-      <c r="C43" s="30"/>
+      <c r="C43" s="29"/>
       <c r="D43" s="11"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>11</v>
       </c>
-      <c r="B44" s="30">
+      <c r="B44" s="29">
         <f>((C4+C18)*1.11) + ((C5+C18)*1.11)</f>
         <v>155.4</v>
       </c>
-      <c r="C44" s="30"/>
+      <c r="C44" s="29"/>
       <c r="D44" s="11"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>12</v>
       </c>
-      <c r="B45" s="30">
+      <c r="B45" s="29">
         <f>((C6+C21)*1.12) + ((C7+C21)*1.12)</f>
         <v>392</v>
       </c>
-      <c r="C45" s="30"/>
+      <c r="C45" s="29"/>
       <c r="D45" s="11"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>13</v>
       </c>
-      <c r="B46" s="30">
+      <c r="B46" s="29">
         <f>((C6+C21)*1.13) + ((C7+C21)*1.13)</f>
         <v>395.5</v>
       </c>
-      <c r="C46" s="30"/>
+      <c r="C46" s="29"/>
       <c r="D46" s="11"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>14</v>
       </c>
-      <c r="B47" s="30">
+      <c r="B47" s="29">
         <f>((C6+C21)*1.14) + ((C7+C21)*1.14)</f>
         <v>399</v>
       </c>
-      <c r="C47" s="30"/>
+      <c r="C47" s="29"/>
       <c r="D47" s="11"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>15</v>
       </c>
-      <c r="B48" s="30">
+      <c r="B48" s="29">
         <f>((C6+C21)*1.15) + ((C7+C21)*1.15)</f>
         <v>402.5</v>
       </c>
-      <c r="C48" s="30"/>
+      <c r="C48" s="29"/>
       <c r="D48" s="11"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>16</v>
       </c>
-      <c r="B49" s="30">
+      <c r="B49" s="29">
         <f>((C6+C21)*1.16) + ((C7+C21)*1.16)</f>
         <v>406</v>
       </c>
-      <c r="C49" s="30"/>
+      <c r="C49" s="29"/>
       <c r="D49" s="11"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="B50" s="31">
-        <v>470</v>
-      </c>
-      <c r="C50" s="31"/>
+      <c r="B50" s="35">
+        <f>SUM(B34:B40)</f>
+        <v>761.7</v>
+      </c>
+      <c r="C50" s="35"/>
       <c r="D50" s="11"/>
-      <c r="E50" s="29"/>
-      <c r="F50" s="29"/>
-      <c r="G50" s="29"/>
-      <c r="H50" s="29"/>
+      <c r="E50" s="34"/>
+      <c r="F50" s="34"/>
+      <c r="G50" s="34"/>
+      <c r="H50" s="34"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="B51" s="32">
-        <f>SUM(B34:B43)</f>
-        <v>1219.5</v>
-      </c>
-      <c r="C51" s="32"/>
+      <c r="B51" s="36">
+        <f>SUM(B34:B44)</f>
+        <v>1374.9</v>
+      </c>
+      <c r="C51" s="36"/>
       <c r="D51" s="11"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="B52" s="33">
+      <c r="B52" s="37">
         <f>SUM(B34:B49)</f>
         <v>3369.9</v>
       </c>
-      <c r="C52" s="33"/>
+      <c r="C52" s="37"/>
       <c r="D52" s="11"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
@@ -1505,20 +1506,20 @@
         <v>44</v>
       </c>
       <c r="B55" s="20">
-        <v>1220</v>
+        <v>800</v>
       </c>
       <c r="C55" s="20">
-        <f>MIN(20, ROUNDUP(IF(B55&lt;=470, (B55/470)*10, 10 + ((B55-470)/(1219.5-470))*10), 0.5))</f>
-        <v>20</v>
+        <f>MIN(20, ROUNDUP(IF(B55&lt;=B50, (B55/B50)*10, 10 + ((B55-B50)/(B51-B50))*10), 0.5))</f>
+        <v>11</v>
       </c>
       <c r="D55" s="11"/>
-      <c r="E55" s="28" t="s">
+      <c r="E55" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="F55" s="28"/>
-      <c r="G55" s="28"/>
-      <c r="H55" s="28"/>
-      <c r="I55" s="28"/>
+      <c r="F55" s="33"/>
+      <c r="G55" s="33"/>
+      <c r="H55" s="33"/>
+      <c r="I55" s="33"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="24" t="s">
@@ -1526,7 +1527,7 @@
       </c>
       <c r="B56" s="25">
         <f>B50</f>
-        <v>470</v>
+        <v>761.7</v>
       </c>
       <c r="C56" s="25">
         <v>10</v>
@@ -1539,7 +1540,7 @@
       </c>
       <c r="B57" s="25">
         <f>B51</f>
-        <v>1219.5</v>
+        <v>1374.9</v>
       </c>
       <c r="C57" s="25">
         <v>20</v>
@@ -1554,27 +1555,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
     <mergeCell ref="E55:I55"/>
     <mergeCell ref="E50:H50"/>
     <mergeCell ref="B48:C48"/>
@@ -1582,6 +1562,27 @@
     <mergeCell ref="B50:C50"/>
     <mergeCell ref="B51:C51"/>
     <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="A29:C29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>